<commit_message>
Added Email Search Agent and keyword with data api
</commit_message>
<xml_diff>
--- a/Email_Bot_APIs_by_Junaid.xlsx
+++ b/Email_Bot_APIs_by_Junaid.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -338,6 +338,32 @@
   </si>
   <si>
     <t>curl --location 'http://1msg.1point1.in:3001/api/email/bot/search/email-agent/by/user-id/?user_id=6&amp;q=Firdos'</t>
+  </si>
+  <si>
+    <t>Search Email agent or keyword by user id</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/email/bot/search/email-agent/keywords/by/user-id/</t>
+  </si>
+  <si>
+    <t>{
+    "user_id" : 6,
+    "agent_name" : "",
+    "keyword" : "Junaid",
+    "from_date" : "2025-05-13",
+    "to_date" : "2025-05-13"
+}</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/email/bot/search/email-agent/keywords/by/user-id/' \
+--header 'Content-Type: application/json' \
+--data '{
+    "user_id" : 6,
+    "agent_name" : "",
+    "keyword" : "Airline",
+    "from_date" : "2025-05-13",
+    "to_date" : "2025-05-13"
+}'</t>
   </si>
 </sst>
 </file>
@@ -742,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,6 +1013,26 @@
       </c>
       <c r="G18" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>9</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1008,8 +1054,9 @@
     <hyperlink ref="D14" r:id="rId6"/>
     <hyperlink ref="D16" r:id="rId7"/>
     <hyperlink ref="D18" r:id="rId8"/>
+    <hyperlink ref="D20" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added manually send Email API , Trigger FetChMailController By Agent Id , Filter Email by Agent_id and from_date and to_date API
</commit_message>
<xml_diff>
--- a/Email_Bot_APIs_by_Junaid.xlsx
+++ b/Email_Bot_APIs_by_Junaid.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="61">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -340,29 +340,129 @@
     <t>curl --location 'http://1msg.1point1.in:3001/api/email/bot/search/email-agent/by/user-id/?user_id=6&amp;q=Firdos'</t>
   </si>
   <si>
-    <t>Search Email agent or keyword by user id</t>
-  </si>
-  <si>
-    <t>http://1msg.1point1.in:3001/api/email/bot/search/email-agent/keywords/by/user-id/</t>
+    <t xml:space="preserve">10 - </t>
+  </si>
+  <si>
+    <t>Send Email manually</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/email/bot/manually/reply-to/email/' \
+--header 'Content-Type: application/json' \
+--data-raw '{
+    "agent_id" : 8,
+    "ticket_no" : 2505130037,
+    "from_address" : "airline.demo@1point1.in",
+    "to_addresses" : ["junaid.ansari@1point1.com"],
+    "cc_addresses" : [],
+    "bcc_addresses" : [],
+    "subject" : "Test Reply Mail",
+    "body_html" : "This is a reply test mail",
+    "mailReceiveAt" : "2025-05-14 04:51:39"
+}'</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/email/bot/manually/reply-to/email/</t>
   </si>
   <si>
     <t>{
-    "user_id" : 6,
-    "agent_name" : "",
-    "keyword" : "Junaid",
-    "from_date" : "2025-05-13",
-    "to_date" : "2025-05-13"
+    "agent_id" : 8,
+    "ticket_no" : 2505130037,
+    "from_address" : "airline.demo@1point1.in",
+    "to_addresses" : ["junaid.ansari@1point1.com"],
+    "cc_addresses" : [],
+    "bcc_addresses" : [],
+    "subject" : "Test Reply Mail",
+    "body_html" : "This is a reply test mail",
+    "mailReceiveAt" : "2025-05-14 04:51:39"
 }</t>
   </si>
   <si>
-    <t>curl --location 'http://1msg.1point1.in:3001/api/email/bot/search/email-agent/keywords/by/user-id/' \
+    <t>Trigger Mail Fetching Controller by Agent ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">curl --location 'http://1msg.1point1.in:3001/api/email/bot/email/fetch/controller/auto-mail/' \
 --header 'Content-Type: application/json' \
 --data '{
-    "user_id" : 6,
-    "agent_name" : "",
-    "keyword" : "Airline",
-    "from_date" : "2025-05-13",
-    "to_date" : "2025-05-13"
+    "agent_id" : 12,
+    "action" : "start"
+}'
+</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/email/bot/email/fetch/controller/auto-mail/</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>#To start fetching mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "agent_id" : 24,
+    "action" : "start"
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t># to Stop fetchig Mail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+{
+    "agent_id" : 24,
+    "action" : "stop"
+}
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Search Email with agent id and dates</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/email/bot/filter/email-agent/keywords/by/user-id/http://1msg.1point1.in:3001/api/email/bot/filter/email-agent/keywords/by/user-id/</t>
+  </si>
+  <si>
+    <t>{
+    "agent_id" : 24,
+    "from_date" : "2025-05-14",
+    "to_date" : "2025-05-14"
+}</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/email/bot/filter/email-agent/keywords/by/user-id/' \
+--header 'Content-Type: application/json' \
+--data '{
+    "agent_id" : 24,
+    "from_date" : "2025-05-14",
+    "to_date" : "2025-05-14"
 }'</t>
   </si>
 </sst>
@@ -370,7 +470,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +490,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -768,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1015,24 +1122,64 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="201.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="288" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="C23" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>51</v>
+    </row>
+    <row r="25" spans="1:7" ht="216" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>11</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1054,9 +1201,11 @@
     <hyperlink ref="D14" r:id="rId6"/>
     <hyperlink ref="D16" r:id="rId7"/>
     <hyperlink ref="D18" r:id="rId8"/>
-    <hyperlink ref="D20" r:id="rId9"/>
+    <hyperlink ref="D23" r:id="rId9"/>
+    <hyperlink ref="D25" r:id="rId10"/>
+    <hyperlink ref="D20" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed Filter Agent name get Email body ans status
</commit_message>
<xml_diff>
--- a/Email_Bot_APIs_by_Junaid.xlsx
+++ b/Email_Bot_APIs_by_Junaid.xlsx
@@ -444,14 +444,14 @@
     </r>
   </si>
   <si>
-    <t>Search Email with agent id and dates</t>
-  </si>
-  <si>
     <t>http://1msg.1point1.in:3001/api/email/bot/filter/email-agent/keywords/by/user-id/http://1msg.1point1.in:3001/api/email/bot/filter/email-agent/keywords/by/user-id/</t>
   </si>
   <si>
+    <t>Filter Email with agent id and dates</t>
+  </si>
+  <si>
     <t>{
-    "agent_id" : 24,
+    "agent_name" : "manoj",
     "from_date" : "2025-05-14",
     "to_date" : "2025-05-14"
 }</t>
@@ -460,7 +460,7 @@
     <t>curl --location 'http://1msg.1point1.in:3001/api/email/bot/filter/email-agent/keywords/by/user-id/' \
 --header 'Content-Type: application/json' \
 --data '{
-    "agent_id" : 24,
+    "agent_name" : "manoj",
     "from_date" : "2025-05-14",
     "to_date" : "2025-05-14"
 }'</t>
@@ -877,7 +877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -1127,13 +1127,13 @@
         <v>9</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Added the email report API
</commit_message>
<xml_diff>
--- a/Email_Bot_APIs_by_Junaid.xlsx
+++ b/Email_Bot_APIs_by_Junaid.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="69">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -485,6 +485,30 @@
     "user_id" : 6,
     "agent_id" : 27,
     "agent_status" : false
+}'</t>
+  </si>
+  <si>
+    <t>Email Report ( Dump )</t>
+  </si>
+  <si>
+    <t>http://1msg.1point1.in:3001/api/email/bot/report/emailbot/agent_id/agent_id/</t>
+  </si>
+  <si>
+    <t>{
+    "agent_id" : 28,
+    "report_type" : 1,
+    "from_date" : "2025-05-01",
+    "to_date" : "2025-05-19"
+}</t>
+  </si>
+  <si>
+    <t>curl --location 'http://1msg.1point1.in:3001/api/email/bot/report/emailbot/agent_id/' \
+--header 'Content-Type: application/json' \
+--data '{
+    "agent_id" : 28,
+    "report_type" : 1,
+    "from_date" : "2025-05-01",
+    "to_date" : "2025-05-19"
 }'</t>
   </si>
 </sst>
@@ -897,10 +921,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="33.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1222,6 +1246,26 @@
       </c>
       <c r="G29" s="1" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>13</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1247,8 +1291,9 @@
     <hyperlink ref="D25" r:id="rId10"/>
     <hyperlink ref="D20" r:id="rId11"/>
     <hyperlink ref="D29" r:id="rId12"/>
+    <hyperlink ref="D32" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId13"/>
+  <pageSetup orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>